<commit_message>
Se sube caso de prueba
</commit_message>
<xml_diff>
--- a/se/Trabajo Profesional/Disciplinas/3.Analisis/Casos de Uso/CU01 - Dando de alta deportista/TC01 -Dando de alta deportista.xlsx
+++ b/se/Trabajo Profesional/Disciplinas/3.Analisis/Casos de Uso/CU01 - Dando de alta deportista/TC01 -Dando de alta deportista.xlsx
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>VARIACIONES</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>Verificar que el sistema informa por pantalla que no sean cargado todos los datos</t>
-  </si>
-  <si>
-    <t>Bajo</t>
   </si>
   <si>
     <t>Alta Deportista</t>
@@ -196,18 +193,6 @@
 2. Seleccionar 'New Sportsman'
 3. Dejar algunos datos obligatorios sin cargar
 4. Presionar Save</t>
-  </si>
-  <si>
-    <t>Alta Deportista - Cancelar carga</t>
-  </si>
-  <si>
-    <t>1. Seleccionar 'Sportsman'
-2. Seleccionar 'New Sportsman'
-3. Completar datos obligatorios
-4. Presionar Salir</t>
-  </si>
-  <si>
-    <t>Verificar que el sistema cierra la ventana de Sportsman. No se crea el sportsman.</t>
   </si>
   <si>
     <t>1. Seleccionar 'Sportsman'
@@ -509,55 +494,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="57"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <condense val="0"/>
@@ -901,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -993,17 +930,17 @@
     <row r="3" spans="1:16" ht="75">
       <c r="A3" s="11"/>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>15</v>
@@ -1021,17 +958,17 @@
     <row r="4" spans="1:16" ht="120">
       <c r="A4" s="11"/>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>15</v>
@@ -1049,11 +986,11 @@
     <row r="5" spans="1:16" ht="60">
       <c r="A5" s="11"/>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>16</v>
@@ -1076,26 +1013,16 @@
       <c r="O5" s="10"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16" ht="60">
+    <row r="6" spans="1:16">
       <c r="A6" s="11"/>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="16"/>
       <c r="J6" s="1"/>
       <c r="K6" s="19"/>
       <c r="L6" s="13"/>
@@ -1115,36 +1042,18 @@
       <c r="H7" s="3"/>
       <c r="I7" s="16"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="19"/>
+      <c r="K7" s="7"/>
       <c r="L7" s="13"/>
       <c r="M7" s="18"/>
       <c r="N7" s="17"/>
       <c r="O7" s="10"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="11"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="1"/>
-    </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="J12:P13 K14:P19 K20:O20 H3:I25 K3:P11" name="datos variaciones"/>
+    <protectedRange sqref="J11:P12 K13:P18 K19:O19 K3:P10 H3:I24" name="datos variaciones"/>
     <protectedRange sqref="H2:J2" name="encabezado variaciones"/>
-    <protectedRange sqref="F1048570:F1048576 A3:G25" name="Datos basicos TC"/>
+    <protectedRange sqref="F1048569:F1048576 A3:G24" name="Datos basicos TC"/>
   </protectedRanges>
   <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
@@ -1152,19 +1061,19 @@
     <mergeCell ref="K1:O1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="G2:G8">
-    <cfRule type="cellIs" dxfId="7" priority="210" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="G2:G7">
+    <cfRule type="cellIs" dxfId="3" priority="210" stopIfTrue="1" operator="equal">
       <formula>"True"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="211" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="211" stopIfTrue="1" operator="equal">
       <formula>"False"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N8">
-    <cfRule type="cellIs" dxfId="5" priority="208" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="N2:N7">
+    <cfRule type="cellIs" dxfId="1" priority="208" stopIfTrue="1" operator="equal">
       <formula>"TEST OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="209" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="209" stopIfTrue="1" operator="equal">
       <formula>"TEST FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1178,7 +1087,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="iconSet" priority="9">
+    <cfRule type="iconSet" priority="6">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1187,15 +1096,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="iconSet" priority="6">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
     <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -1214,16 +1114,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M7">
       <formula1>"Sin ejecutar,Ejecutado,No aplica"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N7">
       <formula1>"TEST OK, TEST FAIL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E7">
       <formula1>"Critico,Alto,Bajo"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G7">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>